<commit_message>
debug koperasi and import
</commit_message>
<xml_diff>
--- a/public/uploads/excel/productList.xlsx
+++ b/public/uploads/excel/productList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F7E5B2-85ED-4440-AF15-8E600F3C2154}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AE5ABA-8EF7-4CBD-991B-A3FB581B9161}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>name</t>
   </si>
@@ -29,15 +29,6 @@
   </si>
   <si>
     <t>price</t>
-  </si>
-  <si>
-    <t>Buku Latihan Math T1</t>
-  </si>
-  <si>
-    <t>Buku Latihan Sains T1</t>
-  </si>
-  <si>
-    <t>Buku Latihan English T1</t>
   </si>
 </sst>
 </file>
@@ -73,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,10 +347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -375,36 +367,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>3.1415899999999999</v>
       </c>
       <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
+        <v>-1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>